<commit_message>
Updated ESP model - 2025-08-19 18:22
</commit_message>
<xml_diff>
--- a/VerveStacks_ESP/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_ESP/ReportDefs_vervestacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F722313C-51C9-4AE2-9912-CBFFFD05F5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B57AB34-5327-4613-BD06-2FC1B690AD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,15 @@
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
     <sheet name="TS_Defs" sheetId="27" r:id="rId2"/>
     <sheet name="TS_ratios" sheetId="68" r:id="rId3"/>
-    <sheet name="PSet_MAP coarse" sheetId="57" r:id="rId4"/>
-    <sheet name="CSET_MAP" sheetId="66" r:id="rId5"/>
-    <sheet name="CName_MAP" sheetId="58" r:id="rId6"/>
-    <sheet name="timeslice map" sheetId="64" r:id="rId7"/>
-    <sheet name="process map" sheetId="65" r:id="rId8"/>
-    <sheet name="commodity map" sheetId="67" r:id="rId9"/>
-    <sheet name="ATS" sheetId="63" r:id="rId10"/>
-    <sheet name="UnitConv" sheetId="59" r:id="rId11"/>
+    <sheet name="Sankey" sheetId="69" r:id="rId4"/>
+    <sheet name="PSet_MAP" sheetId="57" r:id="rId5"/>
+    <sheet name="CSET_MAP" sheetId="66" r:id="rId6"/>
+    <sheet name="CName_MAP" sheetId="58" r:id="rId7"/>
+    <sheet name="timeslice map" sheetId="64" r:id="rId8"/>
+    <sheet name="process map" sheetId="65" r:id="rId9"/>
+    <sheet name="commodity map" sheetId="67" r:id="rId10"/>
+    <sheet name="ATS" sheetId="63" r:id="rId11"/>
+    <sheet name="UnitConv" sheetId="59" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TS_Defs!$A$2:$N$2</definedName>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="257">
   <si>
     <t>Unit</t>
   </si>
@@ -91,12 +92,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Hydro</t>
-  </si>
-  <si>
-    <t>Nuclear</t>
-  </si>
-  <si>
     <t>Solar</t>
   </si>
   <si>
@@ -379,15 +374,9 @@
     <t>Wind offshore</t>
   </si>
   <si>
-    <t>Geothermal</t>
-  </si>
-  <si>
     <t>Hydro pumped stg</t>
   </si>
   <si>
-    <t>Bioenergy</t>
-  </si>
-  <si>
     <t>Util Batt Stg</t>
   </si>
   <si>
@@ -451,9 +440,6 @@
     <t>-ElcAgg*,-*EV*</t>
   </si>
   <si>
-    <t>ELC,ELC_???-???</t>
-  </si>
-  <si>
     <t>t</t>
   </si>
   <si>
@@ -487,160 +473,385 @@
     <t>timeslice</t>
   </si>
   <si>
-    <t>Delayed transition</t>
-  </si>
-  <si>
-    <t>Net Zero 2050</t>
+    <t>Low demand</t>
+  </si>
+  <si>
+    <t>Fragmented World</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>15 days</t>
+  </si>
+  <si>
+    <t>2 weeks</t>
+  </si>
+  <si>
+    <t>_3d</t>
+  </si>
+  <si>
+    <t>_15d</t>
+  </si>
+  <si>
+    <t>_2w</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CO2Captured</t>
+  </si>
+  <si>
+    <t>kt</t>
+  </si>
+  <si>
+    <t>ktneg</t>
+  </si>
+  <si>
+    <t>CO2_emission</t>
+  </si>
+  <si>
+    <t>CO2_captured</t>
+  </si>
+  <si>
+    <t>mt</t>
+  </si>
+  <si>
+    <t>Coal CCS</t>
+  </si>
+  <si>
+    <t>Gas CCS</t>
+  </si>
+  <si>
+    <t>Coal CCS Retrofit</t>
+  </si>
+  <si>
+    <t>Gas CCS Retrofit</t>
+  </si>
+  <si>
+    <t>coal</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>co2captured</t>
+  </si>
+  <si>
+    <t>*ccs-rf</t>
+  </si>
+  <si>
+    <t>co2net</t>
+  </si>
+  <si>
+    <t>000$/t</t>
+  </si>
+  <si>
+    <t>Price_CO2</t>
+  </si>
+  <si>
+    <t>$/tCO2</t>
+  </si>
+  <si>
+    <t>ELE,STG,IRE,-Grid</t>
+  </si>
+  <si>
+    <t>s?a*</t>
+  </si>
+  <si>
+    <t>*,-s?a*</t>
+  </si>
+  <si>
+    <t>hourly</t>
+  </si>
+  <si>
+    <t>aggregated</t>
+  </si>
+  <si>
+    <t>ts_type</t>
+  </si>
+  <si>
+    <t>ts_season</t>
+  </si>
+  <si>
+    <t>S1*</t>
+  </si>
+  <si>
+    <t>S2*</t>
+  </si>
+  <si>
+    <t>S3*</t>
+  </si>
+  <si>
+    <t>S4*</t>
+  </si>
+  <si>
+    <t>S5*</t>
+  </si>
+  <si>
+    <t>S6*</t>
+  </si>
+  <si>
+    <t>~Timeslice_Map</t>
+  </si>
+  <si>
+    <t>vstacks_ts16~</t>
+  </si>
+  <si>
+    <t>vstacks_t_annual~</t>
+  </si>
+  <si>
+    <t>ts-16</t>
+  </si>
+  <si>
+    <t>ts-annual</t>
+  </si>
+  <si>
+    <t>_16</t>
+  </si>
+  <si>
+    <t>_ann</t>
+  </si>
+  <si>
+    <t>-ElcAgg*,-*EV*,-g[_]*</t>
+  </si>
+  <si>
+    <t>ELC,ELC_???-???,e[_]*</t>
+  </si>
+  <si>
+    <t>T_neg_andor</t>
+  </si>
+  <si>
+    <t>downscale_option</t>
+  </si>
+  <si>
+    <t>~TS_Defs: Snk_attr=Grid Flows</t>
+  </si>
+  <si>
+    <t>TWh</t>
+  </si>
+  <si>
+    <t>VAR_FIN</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Elec-220V</t>
+  </si>
+  <si>
+    <t>Elec-400V</t>
+  </si>
+  <si>
+    <t>Elec-380V</t>
+  </si>
+  <si>
+    <t>Elec-225V</t>
+  </si>
+  <si>
+    <t>Elec-330V</t>
+  </si>
+  <si>
+    <t>Elec-275V</t>
+  </si>
+  <si>
+    <t>Elec-420V</t>
+  </si>
+  <si>
+    <t>Elec-300V</t>
+  </si>
+  <si>
+    <t>Elec-500V</t>
+  </si>
+  <si>
+    <t>Elec-750V</t>
+  </si>
+  <si>
+    <t>Elec-450V</t>
+  </si>
+  <si>
+    <t>Elec-515V</t>
+  </si>
+  <si>
+    <t>Elec-525V</t>
+  </si>
+  <si>
+    <t>Elec-320V</t>
+  </si>
+  <si>
+    <t>Elec-150V</t>
+  </si>
+  <si>
+    <t>Elec-270V</t>
+  </si>
+  <si>
+    <t>Elec-350V</t>
+  </si>
+  <si>
+    <t>Elec-250V</t>
+  </si>
+  <si>
+    <t>Elec-200V</t>
+  </si>
+  <si>
+    <t>Elec-236V</t>
+  </si>
+  <si>
+    <t>Elec-600V</t>
+  </si>
+  <si>
+    <t>bioenergy</t>
+  </si>
+  <si>
+    <t>hydrogen</t>
+  </si>
+  <si>
+    <t>nuclear</t>
+  </si>
+  <si>
+    <t>ELC</t>
+  </si>
+  <si>
+    <t>buildings</t>
+  </si>
+  <si>
+    <t>industry</t>
+  </si>
+  <si>
+    <t>transport</t>
+  </si>
+  <si>
+    <t>EVs</t>
+  </si>
+  <si>
+    <t>&lt;cset&gt;_Src_&lt;pset&gt;</t>
+  </si>
+  <si>
+    <t>&lt;cset&gt;_Snk_&lt;pset&gt;</t>
+  </si>
+  <si>
+    <t>fossil</t>
+  </si>
+  <si>
+    <t>Bio Power</t>
+  </si>
+  <si>
+    <t>Solar Util</t>
+  </si>
+  <si>
+    <t>Geothermal P</t>
+  </si>
+  <si>
+    <t>Hydro RoR</t>
+  </si>
+  <si>
+    <t>Nuclear P</t>
+  </si>
+  <si>
+    <t>Nuclear SMR</t>
+  </si>
+  <si>
+    <t>Hydro Dam</t>
+  </si>
+  <si>
+    <t>Solar elec</t>
+  </si>
+  <si>
+    <t>Wind elec</t>
+  </si>
+  <si>
+    <t>renewable</t>
+  </si>
+  <si>
+    <t>Grid-220V</t>
+  </si>
+  <si>
+    <t>Grid-400V</t>
+  </si>
+  <si>
+    <t>Grid-380V</t>
+  </si>
+  <si>
+    <t>Grid-225V</t>
+  </si>
+  <si>
+    <t>Grid-330V</t>
+  </si>
+  <si>
+    <t>Grid-275V</t>
+  </si>
+  <si>
+    <t>Grid-420V</t>
+  </si>
+  <si>
+    <t>Grid-300V</t>
+  </si>
+  <si>
+    <t>Grid-500V</t>
+  </si>
+  <si>
+    <t>Grid-750V</t>
+  </si>
+  <si>
+    <t>Grid-450V</t>
+  </si>
+  <si>
+    <t>Grid-515V</t>
+  </si>
+  <si>
+    <t>Grid-525V</t>
+  </si>
+  <si>
+    <t>Grid-320V</t>
+  </si>
+  <si>
+    <t>Grid-150V</t>
+  </si>
+  <si>
+    <t>Grid-270V</t>
+  </si>
+  <si>
+    <t>Grid-350V</t>
+  </si>
+  <si>
+    <t>Grid-250V</t>
+  </si>
+  <si>
+    <t>Grid-200V</t>
+  </si>
+  <si>
+    <t>Grid-236V</t>
+  </si>
+  <si>
+    <t>Grid-600V</t>
+  </si>
+  <si>
+    <t>Aggregators</t>
+  </si>
+  <si>
+    <t>DUMMY_IMP</t>
+  </si>
+  <si>
+    <t>Transformers Dn</t>
+  </si>
+  <si>
+    <t>Transformers Up</t>
+  </si>
+  <si>
+    <t>Declared NDCs</t>
+  </si>
+  <si>
+    <t>Limited to 2 deg</t>
+  </si>
+  <si>
+    <t>Postponed Transition</t>
+  </si>
+  <si>
+    <t>Target Net Zero 2050</t>
   </si>
   <si>
     <t>Current Policies</t>
-  </si>
-  <si>
-    <t>Low demand</t>
-  </si>
-  <si>
-    <t>Fragmented World</t>
-  </si>
-  <si>
-    <t>NDCs</t>
-  </si>
-  <si>
-    <t>Below 2deg</t>
-  </si>
-  <si>
-    <t>3 days</t>
-  </si>
-  <si>
-    <t>15 days</t>
-  </si>
-  <si>
-    <t>2 weeks</t>
-  </si>
-  <si>
-    <t>_3d</t>
-  </si>
-  <si>
-    <t>_15d</t>
-  </si>
-  <si>
-    <t>_2w</t>
-  </si>
-  <si>
-    <t>CO2</t>
-  </si>
-  <si>
-    <t>CO2Captured</t>
-  </si>
-  <si>
-    <t>kt</t>
-  </si>
-  <si>
-    <t>ktneg</t>
-  </si>
-  <si>
-    <t>CO2_emission</t>
-  </si>
-  <si>
-    <t>CO2_captured</t>
-  </si>
-  <si>
-    <t>mt</t>
-  </si>
-  <si>
-    <t>Coal CCS</t>
-  </si>
-  <si>
-    <t>Gas CCS</t>
-  </si>
-  <si>
-    <t>Coal CCS Retrofit</t>
-  </si>
-  <si>
-    <t>Gas CCS Retrofit</t>
-  </si>
-  <si>
-    <t>coal</t>
-  </si>
-  <si>
-    <t>gas</t>
-  </si>
-  <si>
-    <t>co2captured</t>
-  </si>
-  <si>
-    <t>*ccs-rf</t>
-  </si>
-  <si>
-    <t>co2net</t>
-  </si>
-  <si>
-    <t>000$/t</t>
-  </si>
-  <si>
-    <t>Price_CO2</t>
-  </si>
-  <si>
-    <t>$/tCO2</t>
-  </si>
-  <si>
-    <t>ELE,STG,IRE,-Grid</t>
-  </si>
-  <si>
-    <t>s?a*</t>
-  </si>
-  <si>
-    <t>*,-s?a*</t>
-  </si>
-  <si>
-    <t>hourly</t>
-  </si>
-  <si>
-    <t>aggregated</t>
-  </si>
-  <si>
-    <t>ts_type</t>
-  </si>
-  <si>
-    <t>ts_season</t>
-  </si>
-  <si>
-    <t>S1*</t>
-  </si>
-  <si>
-    <t>S2*</t>
-  </si>
-  <si>
-    <t>S3*</t>
-  </si>
-  <si>
-    <t>S4*</t>
-  </si>
-  <si>
-    <t>S5*</t>
-  </si>
-  <si>
-    <t>S6*</t>
-  </si>
-  <si>
-    <t>~Timeslice_Map</t>
-  </si>
-  <si>
-    <t>vstacks_ts16~</t>
-  </si>
-  <si>
-    <t>vstacks_t_annual~</t>
-  </si>
-  <si>
-    <t>ts-16</t>
-  </si>
-  <si>
-    <t>ts-annual</t>
-  </si>
-  <si>
-    <t>_16</t>
-  </si>
-  <si>
-    <t>_ann</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1399,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="14.25"/>
@@ -1206,43 +1417,43 @@
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="H2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1251,10 +1462,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5" t="str">
         <f>"sg_"&amp;H2</f>
@@ -1272,23 +1483,23 @@
       </c>
       <c r="B6" t="str">
         <f>G6</f>
-        <v>Delayed transition_3d</v>
+        <v>Postponed Transition_3d</v>
       </c>
       <c r="G6" t="str">
         <f>H6&amp;P6</f>
-        <v>Delayed transition_3d</v>
+        <v>Postponed Transition_3d</v>
       </c>
       <c r="H6" t="s">
-        <v>135</v>
+        <v>254</v>
       </c>
       <c r="I6" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1298,23 +1509,23 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" ref="B7:B26" si="1">G7</f>
-        <v>Net Zero 2050_3d</v>
+        <v>Target Net Zero 2050_3d</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" ref="G7:G26" si="2">H7&amp;P7</f>
-        <v>Net Zero 2050_3d</v>
+        <v>Target Net Zero 2050_3d</v>
       </c>
       <c r="H7" t="s">
-        <v>136</v>
+        <v>255</v>
       </c>
       <c r="I7" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N7">
         <v>2</v>
       </c>
       <c r="P7" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1324,23 +1535,23 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>NDCs_3d</v>
+        <v>Declared NDCs_3d</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="2"/>
-        <v>NDCs_3d</v>
+        <v>Declared NDCs_3d</v>
       </c>
       <c r="H8" t="s">
-        <v>140</v>
+        <v>252</v>
       </c>
       <c r="I8" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1350,23 +1561,23 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
-        <v>Below 2deg_3d</v>
+        <v>Limited to 2 deg_3d</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="2"/>
-        <v>Below 2deg_3d</v>
+        <v>Limited to 2 deg_3d</v>
       </c>
       <c r="H9" t="s">
-        <v>141</v>
+        <v>253</v>
       </c>
       <c r="I9" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N9">
         <v>4</v>
       </c>
       <c r="P9" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1383,16 +1594,16 @@
         <v>Current Policies_3d</v>
       </c>
       <c r="H10" t="s">
-        <v>137</v>
+        <v>256</v>
       </c>
       <c r="I10" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N10">
         <v>5</v>
       </c>
       <c r="P10" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1409,16 +1620,16 @@
         <v>Low demand_3d</v>
       </c>
       <c r="H11" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="I11" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N11">
         <v>6</v>
       </c>
       <c r="P11" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1435,16 +1646,16 @@
         <v>Fragmented World_3d</v>
       </c>
       <c r="H12" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="I12" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N12">
         <v>7</v>
       </c>
       <c r="P12" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1454,25 +1665,25 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" si="1"/>
-        <v>Delayed transition_15d</v>
+        <v>Postponed Transition_15d</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
-        <v>Delayed transition_15d</v>
+        <v>Postponed Transition_15d</v>
       </c>
       <c r="H13" t="str">
         <f>H6</f>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I13" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N13">
         <f>N6</f>
         <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1482,25 +1693,25 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" si="1"/>
-        <v>Net Zero 2050_15d</v>
+        <v>Target Net Zero 2050_15d</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="2"/>
-        <v>Net Zero 2050_15d</v>
+        <v>Target Net Zero 2050_15d</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" ref="H14:H41" si="4">H7</f>
-        <v>Net Zero 2050</v>
+        <f t="shared" ref="H14:H40" si="4">H7</f>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N14">
         <f t="shared" ref="N14:N40" si="5">N7</f>
         <v>2</v>
       </c>
       <c r="P14" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1510,25 +1721,25 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" si="1"/>
-        <v>NDCs_15d</v>
+        <v>Declared NDCs_15d</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="2"/>
-        <v>NDCs_15d</v>
+        <v>Declared NDCs_15d</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I15" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1538,25 +1749,25 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" si="1"/>
-        <v>Below 2deg_15d</v>
+        <v>Limited to 2 deg_15d</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="2"/>
-        <v>Below 2deg_15d</v>
+        <v>Limited to 2 deg_15d</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I16" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P16" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1577,14 +1788,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I17" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P17" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1605,14 +1816,14 @@
         <v>Low demand</v>
       </c>
       <c r="I18" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P18" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1633,14 +1844,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I19" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P19" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1650,25 +1861,25 @@
       </c>
       <c r="B20" t="str">
         <f t="shared" si="1"/>
-        <v>Delayed transition_2w</v>
+        <v>Postponed Transition_2w</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="2"/>
-        <v>Delayed transition_2w</v>
+        <v>Postponed Transition_2w</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="4"/>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I20" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N20">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P20" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1678,25 +1889,25 @@
       </c>
       <c r="B21" t="str">
         <f t="shared" si="1"/>
-        <v>Net Zero 2050_2w</v>
+        <v>Target Net Zero 2050_2w</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="2"/>
-        <v>Net Zero 2050_2w</v>
+        <v>Target Net Zero 2050_2w</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="4"/>
-        <v>Net Zero 2050</v>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I21" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P21" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1706,25 +1917,25 @@
       </c>
       <c r="B22" t="str">
         <f t="shared" si="1"/>
-        <v>NDCs_2w</v>
+        <v>Declared NDCs_2w</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="2"/>
-        <v>NDCs_2w</v>
+        <v>Declared NDCs_2w</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I22" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P22" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1734,25 +1945,25 @@
       </c>
       <c r="B23" t="str">
         <f t="shared" si="1"/>
-        <v>Below 2deg_2w</v>
+        <v>Limited to 2 deg_2w</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="2"/>
-        <v>Below 2deg_2w</v>
+        <v>Limited to 2 deg_2w</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I23" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N23">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P23" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1773,14 +1984,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I24" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P24" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1801,14 +2012,14 @@
         <v>Low demand</v>
       </c>
       <c r="I25" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P25" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1829,14 +2040,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I26" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N26">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P26" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1845,54 +2056,54 @@
         <v>vstacks_ts16~0001</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" ref="B27:B41" si="7">G27</f>
-        <v>Delayed transition_16</v>
+        <f t="shared" ref="B27:B40" si="7">G27</f>
+        <v>Postponed Transition_16</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G41" si="8">H27&amp;P27</f>
-        <v>Delayed transition_16</v>
+        <f t="shared" ref="G27:G40" si="8">H27&amp;P27</f>
+        <v>Postponed Transition_16</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="4"/>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I27" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N27">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P27" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" t="str">
-        <f t="shared" ref="A28:A40" si="9">$D$1&amp;TEXT(N28,"0000")</f>
+        <f t="shared" ref="A28:A33" si="9">$D$1&amp;TEXT(N28,"0000")</f>
         <v>vstacks_ts16~0002</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="7"/>
-        <v>Net Zero 2050_16</v>
+        <v>Target Net Zero 2050_16</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="8"/>
-        <v>Net Zero 2050_16</v>
+        <v>Target Net Zero 2050_16</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="4"/>
-        <v>Net Zero 2050</v>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I28" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N28">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P28" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1902,25 +2113,25 @@
       </c>
       <c r="B29" t="str">
         <f t="shared" si="7"/>
-        <v>NDCs_16</v>
+        <v>Declared NDCs_16</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="8"/>
-        <v>NDCs_16</v>
+        <v>Declared NDCs_16</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I29" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N29">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P29" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -1930,25 +2141,25 @@
       </c>
       <c r="B30" t="str">
         <f t="shared" si="7"/>
-        <v>Below 2deg_16</v>
+        <v>Limited to 2 deg_16</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="8"/>
-        <v>Below 2deg_16</v>
+        <v>Limited to 2 deg_16</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I30" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N30">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P30" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -1969,14 +2180,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I31" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N31">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P31" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -1997,14 +2208,14 @@
         <v>Low demand</v>
       </c>
       <c r="I32" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N32">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P32" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2025,14 +2236,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I33" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="N33">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P33" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2042,25 +2253,25 @@
       </c>
       <c r="B34" t="str">
         <f t="shared" si="7"/>
-        <v>Delayed transition_ann</v>
+        <v>Postponed Transition_ann</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="8"/>
-        <v>Delayed transition_ann</v>
+        <v>Postponed Transition_ann</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="4"/>
-        <v>Delayed transition</v>
+        <v>Postponed Transition</v>
       </c>
       <c r="I34" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N34">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P34" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -2070,25 +2281,25 @@
       </c>
       <c r="B35" t="str">
         <f t="shared" si="7"/>
-        <v>Net Zero 2050_ann</v>
+        <v>Target Net Zero 2050_ann</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="8"/>
-        <v>Net Zero 2050_ann</v>
+        <v>Target Net Zero 2050_ann</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="4"/>
-        <v>Net Zero 2050</v>
+        <v>Target Net Zero 2050</v>
       </c>
       <c r="I35" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N35">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="P35" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -2098,25 +2309,25 @@
       </c>
       <c r="B36" t="str">
         <f t="shared" si="7"/>
-        <v>NDCs_ann</v>
+        <v>Declared NDCs_ann</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="8"/>
-        <v>NDCs_ann</v>
+        <v>Declared NDCs_ann</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="4"/>
-        <v>NDCs</v>
+        <v>Declared NDCs</v>
       </c>
       <c r="I36" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N36">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="P36" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -2126,25 +2337,25 @@
       </c>
       <c r="B37" t="str">
         <f t="shared" si="7"/>
-        <v>Below 2deg_ann</v>
+        <v>Limited to 2 deg_ann</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="8"/>
-        <v>Below 2deg_ann</v>
+        <v>Limited to 2 deg_ann</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="4"/>
-        <v>Below 2deg</v>
+        <v>Limited to 2 deg</v>
       </c>
       <c r="I37" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N37">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P37" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -2165,14 +2376,14 @@
         <v>Current Policies</v>
       </c>
       <c r="I38" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N38">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P38" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -2193,14 +2404,14 @@
         <v>Low demand</v>
       </c>
       <c r="I39" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N39">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P39" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -2221,14 +2432,14 @@
         <v>Fragmented World</v>
       </c>
       <c r="I40" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="N40">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P40" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2239,6 +2450,60 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3245E1-8745-41DD-8AE6-2F4FA19D9F1C}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G3"/>
@@ -2252,30 +2517,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2286,7 +2551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet31"/>
   <dimension ref="A1:D7"/>
@@ -2310,32 +2575,32 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <f>1/8.76</f>
@@ -2344,13 +2609,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D4">
         <f>1/8.76*100</f>
@@ -2359,13 +2624,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D5">
         <v>1E-3</v>
@@ -2373,13 +2638,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D6">
         <v>-1E-3</v>
@@ -2387,13 +2652,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D7">
         <v>-1000</v>
@@ -2411,7 +2676,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -2442,48 +2707,48 @@
   <sheetData>
     <row r="1" spans="1:21" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>2</v>
@@ -2492,226 +2757,226 @@
         <v>1</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="K3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="U4" s="8"/>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="I5" t="s">
-        <v>123</v>
+        <v>178</v>
       </c>
       <c r="K5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="N5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D6" s="2"/>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="K7" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="N7" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="K8" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="N8" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N10" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q10" t="s">
         <v>48</v>
-      </c>
-      <c r="P10" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="K11" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="N11" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P12" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q12" t="s">
         <v>51</v>
-      </c>
-      <c r="K12" t="s">
-        <v>87</v>
-      </c>
-      <c r="N12" t="s">
-        <v>52</v>
-      </c>
-      <c r="P12" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2746,15 +3011,15 @@
   <sheetData>
     <row r="1" spans="3:11">
       <c r="C1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="3:11">
       <c r="C2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -2763,42 +3028,42 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="3:11">
       <c r="C3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2809,35 +3074,584 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D44EBE-400A-4EA2-9DA1-076783A77DFC}">
+  <dimension ref="A3:S6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="30.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.53125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.53125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.9296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:19" ht="17.25" thickBot="1">
+      <c r="A3" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" thickTop="1" thickBot="1">
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
+        <v>CCGT,Int Comb,Gas_Oil Steam,OCGT (Peaker),Subcritical Coal,Supercritical Coal,IGCC,Bio Power,Solar Util,Wind onshore,Wind offshore,Geothermal P,Hydro Dam,Hydro RoR,Nuclear P,Nuclear SMR,Hydro pumped stg,Util Batt Stg,EV Batt,Demand,Transformers Dn,Transformers Up,Grid-220V,Grid-400V,Grid-380V,Grid-225V,Grid-330V,Grid-275V,Grid-420V,Grid-300V,Grid-500V,Grid-750V,Grid-450V,Grid-515V,Grid-525V,Grid-320V,Grid-150V,Grid-270V,Grid-350V,Grid-250V,Grid-200V,Grid-236V,Grid-600V,Aggregators,DUMMY_IMP</v>
+      </c>
+      <c r="G5" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,CSET_MAP!$A$3:$A$43)</f>
+        <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
+      </c>
+      <c r="J5" t="s">
+        <v>182</v>
+      </c>
+      <c r="M5" t="s">
+        <v>214</v>
+      </c>
+      <c r="S5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,PSet_MAP!$A$3:$A$49)</f>
+        <v>CCGT,Int Comb,Gas_Oil Steam,OCGT (Peaker),Subcritical Coal,Supercritical Coal,IGCC,Bio Power,Solar Util,Wind onshore,Wind offshore,Geothermal P,Hydro Dam,Hydro RoR,Nuclear P,Nuclear SMR,Hydro pumped stg,Util Batt Stg,EV Batt,Demand,Transformers Dn,Transformers Up,Grid-220V,Grid-400V,Grid-380V,Grid-225V,Grid-330V,Grid-275V,Grid-420V,Grid-300V,Grid-500V,Grid-750V,Grid-450V,Grid-515V,Grid-525V,Grid-320V,Grid-150V,Grid-270V,Grid-350V,Grid-250V,Grid-200V,Grid-236V,Grid-600V,Aggregators,DUMMY_IMP</v>
+      </c>
+      <c r="G6" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,CSET_MAP!$A$3:$A$43)</f>
+        <v>Elec-220V,Elec-400V,Elec-380V,Elec-225V,Elec-330V,Elec-275V,Elec-420V,Elec-300V,Elec-500V,Elec-750V,Elec-450V,Elec-515V,Elec-525V,Elec-320V,Elec-150V,Elec-270V,Elec-350V,Elec-250V,Elec-200V,Elec-236V,Elec-600V,Solar elec,Wind elec,fossil,renewable,bioenergy,hydrogen,nuclear,ELC,buildings,industry,transport,EVs</v>
+      </c>
+      <c r="J6" t="s">
+        <v>182</v>
+      </c>
+      <c r="M6" t="s">
+        <v>215</v>
+      </c>
+      <c r="S6">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="str">
+        <f>A3</f>
+        <v>CCGT</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B47" si="0">A4</f>
+        <v>Int Comb</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Gas_Oil Steam</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>OCGT (Peaker)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>Subcritical Coal</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>Supercritical Coal</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>IGCC</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>Bio Power</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>Solar Util</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>Wind onshore</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>Wind offshore</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>Geothermal P</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro Dam</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>220</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro RoR</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>Nuclear P</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>Nuclear SMR</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro pumped stg</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>Util Batt Stg</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>EV Batt</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>Demand</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>250</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>Transformers Dn</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>251</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>Transformers Up</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-220V</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>228</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-400V</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>229</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-380V</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>230</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-225V</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>231</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-330V</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>232</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-275V</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>233</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-420V</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-300V</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>235</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-500V</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>236</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-750V</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>237</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-450V</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>238</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-515V</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>239</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-525V</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>240</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-320V</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>241</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-150V</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>242</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-270V</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>243</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-350V</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>244</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-250V</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>245</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-200V</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>246</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-236V</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>247</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-600V</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>248</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>Aggregators</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>249</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>DUMMY_IMP</v>
       </c>
     </row>
   </sheetData>
@@ -2846,12 +3660,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E766D8-7F73-4A5A-98A5-9C85D527817F}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2861,18 +3675,315 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="str">
+        <f>A3</f>
+        <v>Elec-220V</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B35" si="0">A4</f>
+        <v>Elec-400V</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-380V</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-225V</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-330V</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-275V</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-420V</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-300V</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-500V</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-750V</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-450V</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-515V</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-525V</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>198</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-320V</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-150V</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-270V</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-350V</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-250V</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>203</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-200V</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-236V</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>Elec-600V</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>224</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>Solar elec</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>Wind elec</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>216</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>fossil</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>226</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>renewable</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>bioenergy</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>hydrogen</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>nuclear</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>209</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>ELC</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>buildings</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>211</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>industry</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>212</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>transport</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>213</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>EVs</v>
       </c>
     </row>
   </sheetData>
@@ -2880,7 +3991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C2"/>
@@ -2900,18 +4011,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2920,7 +4031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32957E82-8232-40A9-A839-CC5F79005B92}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C10"/>
@@ -2938,48 +4049,48 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C5" t="str">
         <f>LEFT(B5,2)</f>
@@ -2988,10 +4099,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ref="C6:C10" si="0">LEFT(B6,2)</f>
@@ -3000,10 +4111,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -3012,10 +4123,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -3024,10 +4135,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -3036,10 +4147,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -3051,12 +4162,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ADB714-E6AA-4E3E-B77B-62B65BA0E218}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3071,411 +4182,681 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" t="str">
-        <f>D3</f>
-        <v>CCGT</v>
-      </c>
-      <c r="D3" t="s">
-        <v>90</v>
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" ref="C4:C20" si="0">D4</f>
-        <v>Int Comb</v>
-      </c>
-      <c r="D4" t="s">
-        <v>91</v>
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>Gas_Oil Steam</v>
+        <f>D5</f>
+        <v>CCGT</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>Nuclear</v>
+        <f t="shared" ref="C6:C49" si="0">D6</f>
+        <v>Int Comb</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>OCGT (Peaker)</v>
+        <v>Gas_Oil Steam</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>Subcritical Coal</v>
+        <v>OCGT (Peaker)</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>Supercritical Coal</v>
+        <v>Subcritical Coal</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>IGCC</v>
+        <v>Supercritical Coal</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>Bioenergy</v>
+        <v>IGCC</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>Solar</v>
+        <v>Bio Power</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>Wind onshore</v>
+        <v>Solar Util</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>Wind offshore</v>
+        <v>Wind onshore</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>Geothermal</v>
+        <v>Wind offshore</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>Hydro</v>
+        <v>Geothermal P</v>
       </c>
       <c r="D16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro Dam</v>
+      </c>
+      <c r="D17" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro RoR</v>
+      </c>
+      <c r="D18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Nuclear P</v>
+      </c>
+      <c r="D19" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Nuclear SMR</v>
+      </c>
+      <c r="D20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>Hydro pumped stg</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>Util Batt Stg</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>EV Batt</v>
+      </c>
+      <c r="D23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>Demand</v>
+      </c>
+      <c r="D24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Transformers Dn</v>
+      </c>
+      <c r="D25" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>Transformers Up</v>
+      </c>
+      <c r="D26" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-220V</v>
+      </c>
+      <c r="D27" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-400V</v>
+      </c>
+      <c r="D28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-380V</v>
+      </c>
+      <c r="D29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-225V</v>
+      </c>
+      <c r="D30" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-330V</v>
+      </c>
+      <c r="D31" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-275V</v>
+      </c>
+      <c r="D32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-420V</v>
+      </c>
+      <c r="D33" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-300V</v>
+      </c>
+      <c r="D34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-500V</v>
+      </c>
+      <c r="D35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-750V</v>
+      </c>
+      <c r="D36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-450V</v>
+      </c>
+      <c r="D37" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-515V</v>
+      </c>
+      <c r="D38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-525V</v>
+      </c>
+      <c r="D39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-320V</v>
+      </c>
+      <c r="D40" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-150V</v>
+      </c>
+      <c r="D41" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-270V</v>
+      </c>
+      <c r="D42" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-350V</v>
+      </c>
+      <c r="D43" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-250V</v>
+      </c>
+      <c r="D44" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-200V</v>
+      </c>
+      <c r="D45" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-236V</v>
+      </c>
+      <c r="D46" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>Grid-600V</v>
+      </c>
+      <c r="D47" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>Aggregators</v>
+      </c>
+      <c r="D48" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>DUMMY_IMP</v>
+      </c>
+      <c r="D49" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" t="s">
+        <v>145</v>
+      </c>
+      <c r="E50" t="s">
+        <v>149</v>
+      </c>
+      <c r="F50" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" t="s">
+        <v>150</v>
+      </c>
+      <c r="F51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E52" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" t="s">
+        <v>152</v>
+      </c>
+      <c r="C53" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>Nuclear</v>
-      </c>
-      <c r="D17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v>Hydro pumped stg</v>
-      </c>
-      <c r="D18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v>Util Batt Stg</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>EV Batt</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C55" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E21" t="s">
-        <v>159</v>
-      </c>
-      <c r="F21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" t="s">
-        <v>156</v>
-      </c>
-      <c r="E22" t="s">
-        <v>160</v>
-      </c>
-      <c r="F22" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" t="s">
-        <v>157</v>
-      </c>
-      <c r="E23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" t="s">
-        <v>162</v>
-      </c>
-      <c r="C24" t="s">
-        <v>158</v>
-      </c>
-      <c r="E24" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3245E1-8745-41DD-8AE6-2F4FA19D9F1C}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" t="s">
-        <v>81</v>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>